<commit_message>
added Jcamp example mappings
</commit_message>
<xml_diff>
--- a/mappings/MergedMIs.xlsx
+++ b/mappings/MergedMIs.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6300" tabRatio="833" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6300" tabRatio="898" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="9" r:id="rId1"/>
+    <sheet name="Remarks" sheetId="9" r:id="rId1"/>
     <sheet name="NMRsampleDescription" sheetId="8" r:id="rId2"/>
     <sheet name="NMRinstrument" sheetId="1" r:id="rId3"/>
     <sheet name="NMRsample" sheetId="2" r:id="rId4"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
   <si>
     <t>NMRinstrument</t>
   </si>
@@ -302,6 +302,27 @@
   </si>
   <si>
     <t>Notes:</t>
+  </si>
+  <si>
+    <t>OBSERVE FREQUENCY</t>
+  </si>
+  <si>
+    <t>OBSERVE NUCLEUS</t>
+  </si>
+  <si>
+    <t>PULSE SEQUENCE</t>
+  </si>
+  <si>
+    <t>SPECTROMETER/DATA SYSTEM</t>
+  </si>
+  <si>
+    <t>DELAY</t>
+  </si>
+  <si>
+    <t>Bruker TopSpin Parameter</t>
+  </si>
+  <si>
+    <t>Varian vNMR Parameter</t>
   </si>
 </sst>
 </file>
@@ -645,7 +666,7 @@
   <dimension ref="E1:E19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E20"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,24 +733,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C1" activeCellId="2" sqref="A1 B1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,40 +775,46 @@
     <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -779,41 +822,41 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1019,9 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1044,132 +1085,155 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.28515625" customWidth="1"/>
     <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1181,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,12 +1257,21 @@
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1208,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1293,7 @@
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -1230,48 +1303,54 @@
       <c r="C1" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -1283,10 +1362,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,12 +1374,21 @@
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1310,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,12 +1410,21 @@
     <col min="2" max="2" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>